<commit_message>
Restructure networking cost calculator for clarity
Base Network sheet:
- Focus on zone-to-zone data transfer within region
- Same AZ (private IP): Free
- Cross-AZ (same region): $0.01/GB each direction

VPC Peering sheet:
- Focus on costs specific to VPC Peering component
- 01_same_region: No additional peering cost (base rates apply)
- 02_different_region: $0.02/GB peering cost

Summary sheet:
- Updated references and example calculations
- Clear separation of base network vs component costs
</commit_message>
<xml_diff>
--- a/aws/aws_networking_cost_calculator.xlsx
+++ b/aws/aws_networking_cost_calculator.xlsx
@@ -537,7 +537,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
@@ -556,275 +556,197 @@
     <row r="1" ht="18.75" customHeight="1" s="9">
       <c r="A1" s="12" t="inlineStr">
         <is>
-          <t>AWS Base Network Cost Calculator</t>
+          <t>AWS Base Network Data Transfer Costs</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>(Within Region - Zone to Zone)</t>
         </is>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" s="9">
-      <c r="A3" s="8" t="inlineStr">
-        <is>
-          <t>FIXED MONTHLY COSTS</t>
-        </is>
-      </c>
+      <c r="A3" s="8" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Component</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>Unit Rate ($/hr)</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>Hours/Month</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>Formula</t>
-        </is>
-      </c>
-      <c r="F4" s="1" t="inlineStr">
-        <is>
-          <t>Monthly Cost ($)</t>
-        </is>
-      </c>
+          <t>DATA TRANSFER COSTS</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="n"/>
+      <c r="E4" s="1" t="n"/>
+      <c r="F4" s="1" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="11" t="inlineStr">
         <is>
-          <t>NAT Gateway</t>
-        </is>
-      </c>
-      <c r="B5" s="11" t="n">
-        <v>0.045</v>
-      </c>
-      <c r="C5" s="11" t="n">
-        <v>730</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="11">
-        <f>B5*C5*D5</f>
-        <v/>
-      </c>
-      <c r="F5" s="4">
-        <f>B5*C5*D5</f>
-        <v/>
-      </c>
+          <t>Scenario</t>
+        </is>
+      </c>
+      <c r="B5" s="11" t="inlineStr">
+        <is>
+          <t>Rate ($/GB)</t>
+        </is>
+      </c>
+      <c r="C5" s="11" t="inlineStr">
+        <is>
+          <t>Data (GB)</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>Formula</t>
+        </is>
+      </c>
+      <c r="E5" s="11" t="inlineStr">
+        <is>
+          <t>Monthly Cost ($)</t>
+        </is>
+      </c>
+      <c r="F5" s="4" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="11" t="inlineStr">
         <is>
-          <t>Elastic IP (attached to NAT GW)</t>
+          <t>Same AZ (private IP)</t>
         </is>
       </c>
       <c r="B6" s="11" t="n">
         <v>0</v>
       </c>
       <c r="C6" s="11" t="n">
-        <v>730</v>
-      </c>
-      <c r="D6" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="D6" s="3">
+        <f>B6*C6</f>
+        <v/>
+      </c>
       <c r="E6" s="11">
-        <f>B6*C6*D6</f>
-        <v/>
-      </c>
-      <c r="F6" s="4">
-        <f>B6*C6*D6</f>
-        <v/>
-      </c>
+        <f>B6*C6</f>
+        <v/>
+      </c>
+      <c r="F6" s="4" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="10" t="inlineStr">
         <is>
-          <t>Subtotal (Per NAT Gateway)</t>
-        </is>
-      </c>
-      <c r="B7" s="14" t="n"/>
-      <c r="C7" s="14" t="n"/>
-      <c r="D7" s="14" t="n"/>
-      <c r="E7" s="15" t="n"/>
-      <c r="F7" s="5">
-        <f>SUM(F5:F6)</f>
-        <v/>
-      </c>
-    </row>
+          <t>Cross-AZ (same region) - per direction</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f>B7*C7*2</f>
+        <v/>
+      </c>
+      <c r="E7">
+        <f>B7*C7*2</f>
+        <v/>
+      </c>
+      <c r="F7" s="5" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Subtotal</t>
+        </is>
+      </c>
+      <c r="E8">
+        <f>SUM(E6:E7)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9"/>
     <row r="10" ht="15.75" customHeight="1" s="9">
       <c r="A10" s="8" t="inlineStr">
         <is>
-          <t>VARIABLE MONTHLY COSTS</t>
-        </is>
+          <t>TOTAL MONTHLY COST</t>
+        </is>
+      </c>
+      <c r="E10">
+        <f>E8</f>
+        <v/>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Component</t>
-        </is>
-      </c>
-      <c r="B11" s="1" t="inlineStr">
-        <is>
-          <t>Rate ($/GB)</t>
-        </is>
-      </c>
-      <c r="C11" s="1" t="inlineStr">
-        <is>
-          <t>Data (GB)</t>
-        </is>
-      </c>
-      <c r="D11" s="1" t="inlineStr">
-        <is>
-          <t>Formula</t>
-        </is>
-      </c>
-      <c r="E11" s="1" t="inlineStr">
-        <is>
-          <t>Monthly Cost ($)</t>
-        </is>
-      </c>
+      <c r="A11" s="1" t="n"/>
+      <c r="B11" s="1" t="n"/>
+      <c r="C11" s="1" t="n"/>
+      <c r="D11" s="1" t="n"/>
+      <c r="E11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="11" t="inlineStr">
         <is>
-          <t>NAT Gateway Data Processing</t>
-        </is>
-      </c>
-      <c r="B12" s="11" t="n">
-        <v>0.045</v>
-      </c>
-      <c r="C12" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="11">
-        <f>B12*C12</f>
-        <v/>
-      </c>
-      <c r="E12" s="4">
-        <f>B12*C12*D5</f>
-        <v/>
-      </c>
+          <t>Notes:</t>
+        </is>
+      </c>
+      <c r="B12" s="11" t="n"/>
+      <c r="C12" s="3" t="n"/>
+      <c r="D12" s="11" t="n"/>
+      <c r="E12" s="4" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="11" t="inlineStr">
         <is>
-          <t>Data Transfer Out (first 10TB)</t>
-        </is>
-      </c>
-      <c r="B13" s="11" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="C13" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="11">
-        <f>B13*C13</f>
-        <v/>
-      </c>
-      <c r="E13" s="4">
-        <f>B13*C13</f>
-        <v/>
-      </c>
+          <t>• Same AZ with private IP addresses is FREE</t>
+        </is>
+      </c>
+      <c r="B13" s="11" t="n"/>
+      <c r="C13" s="3" t="n"/>
+      <c r="D13" s="11" t="n"/>
+      <c r="E13" s="4" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="11" t="inlineStr">
         <is>
-          <t>Cross-Region Data Transfer</t>
-        </is>
-      </c>
-      <c r="B14" s="11" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="C14" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="11">
-        <f>B14*C14</f>
-        <v/>
-      </c>
-      <c r="E14" s="4">
-        <f>B14*C14</f>
-        <v/>
-      </c>
+          <t>• Cross-AZ is $0.01/GB in EACH direction ($0.02/GB round-trip)</t>
+        </is>
+      </c>
+      <c r="B14" s="11" t="n"/>
+      <c r="C14" s="3" t="n"/>
+      <c r="D14" s="11" t="n"/>
+      <c r="E14" s="4" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="10" t="inlineStr">
         <is>
-          <t>Variable Subtotal</t>
-        </is>
-      </c>
-      <c r="B15" s="14" t="n"/>
-      <c r="C15" s="14" t="n"/>
-      <c r="D15" s="15" t="n"/>
-      <c r="E15" s="5">
-        <f>SUM(E12:E14)</f>
-        <v/>
+          <t>• These are base AWS data transfer costs (no special components)</t>
+        </is>
+      </c>
+      <c r="E15" s="5" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>• Green cells (Data GB) are inputs - modify as needed</t>
+        </is>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1" s="9">
-      <c r="A17" s="13" t="inlineStr">
-        <is>
-          <t>TOTAL MONTHLY COST</t>
-        </is>
-      </c>
-      <c r="B17" s="14" t="n"/>
-      <c r="C17" s="14" t="n"/>
-      <c r="D17" s="14" t="n"/>
-      <c r="E17" s="15" t="n"/>
-      <c r="F17" s="6">
-        <f>F7+E15</f>
-        <v/>
-      </c>
-    </row>
+      <c r="A17" s="13" t="n"/>
+      <c r="F17" s="6" t="n"/>
+    </row>
+    <row r="18"/>
     <row r="19">
-      <c r="A19" s="7" t="inlineStr">
-        <is>
-          <t>Notes:</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>• Green cells are inputs - modify these values</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>• Prices are for us-east-1 region</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>• NAT Gateway Data Processing is multiplied by number of NAT Gateways</t>
-        </is>
-      </c>
-    </row>
+      <c r="A19" s="7" t="n"/>
+    </row>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A17:E17"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -835,7 +757,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:E1"/>
@@ -857,158 +779,158 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>(Costs specific to VPC Peering component)</t>
+        </is>
+      </c>
+    </row>
     <row r="3" ht="15.75" customHeight="1" s="9">
-      <c r="A3" s="8" t="inlineStr">
-        <is>
-          <t>FIXED MONTHLY COSTS</t>
-        </is>
-      </c>
+      <c r="A3" s="8" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Component</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>Rate</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="inlineStr">
-        <is>
-          <t>Formula</t>
-        </is>
-      </c>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>Monthly Cost ($)</t>
-        </is>
-      </c>
+          <t>FIXED COSTS</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="n"/>
+      <c r="E4" s="1" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="11" t="inlineStr">
         <is>
-          <t>VPC Peering Connection</t>
+          <t>Component</t>
         </is>
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="11">
-        <f>0*C5</f>
-        <v/>
-      </c>
-      <c r="E5" s="4">
-        <f>0*C5</f>
-        <v/>
+          <t>Rate</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="D5" s="11" t="inlineStr">
+        <is>
+          <t>Formula</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>Monthly Cost ($)</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="10" t="inlineStr">
         <is>
+          <t>VPC Peering Connection</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f>0*C6</f>
+        <v/>
+      </c>
+      <c r="E6" s="5">
+        <f>0*C6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>Fixed Subtotal</t>
         </is>
       </c>
-      <c r="E6" s="5">
-        <f>SUM(E5:E5)</f>
+      <c r="E7">
+        <f>SUM(E6:E6)</f>
         <v/>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1" s="9">
-      <c r="A8" s="8" t="inlineStr">
-        <is>
-          <t>VARIABLE MONTHLY COSTS</t>
-        </is>
-      </c>
+      <c r="A8" s="8" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Component</t>
-        </is>
-      </c>
-      <c r="B9" s="1" t="inlineStr">
-        <is>
-          <t>Rate ($/GB)</t>
-        </is>
-      </c>
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t>Data (GB)</t>
-        </is>
-      </c>
-      <c r="D9" s="1" t="inlineStr">
-        <is>
-          <t>Formula</t>
-        </is>
-      </c>
-      <c r="E9" s="1" t="inlineStr">
-        <is>
-          <t>Monthly Cost ($)</t>
-        </is>
-      </c>
+          <t>VARIABLE COSTS (VPC Peering specific)</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="n"/>
+      <c r="C9" s="1" t="n"/>
+      <c r="D9" s="1" t="n"/>
+      <c r="E9" s="1" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="11" t="inlineStr">
         <is>
-          <t>01_same_region: Same AZ</t>
-        </is>
-      </c>
-      <c r="B10" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="11">
-        <f>B10*C10</f>
-        <v/>
-      </c>
-      <c r="E10" s="4">
-        <f>B10*C10</f>
-        <v/>
+          <t>Scenario</t>
+        </is>
+      </c>
+      <c r="B10" s="11" t="inlineStr">
+        <is>
+          <t>Peering Cost ($/GB)</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Data (GB)</t>
+        </is>
+      </c>
+      <c r="D10" s="11" t="inlineStr">
+        <is>
+          <t>Formula</t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t>Monthly Cost ($)</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="11" t="inlineStr">
         <is>
-          <t>01_same_region: Cross-AZ</t>
+          <t>01_same_region: Same AZ</t>
         </is>
       </c>
       <c r="B11" s="11" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="11">
-        <f>B11*C11*2</f>
+        <f>B11*C11</f>
         <v/>
       </c>
       <c r="E11" s="4">
-        <f>B11*C11*2</f>
+        <f>B11*C11</f>
         <v/>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>02_different_region: Cross-Region</t>
+          <t>01_same_region: Cross-AZ</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
         <v>1</v>
@@ -1025,68 +947,108 @@
     <row r="13">
       <c r="A13" s="10" t="inlineStr">
         <is>
+          <t>02_different_region: Cross-Region</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f>B13*C13</f>
+        <v/>
+      </c>
+      <c r="E13" s="5">
+        <f>B13*C13</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1" s="9">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>Variable Subtotal</t>
         </is>
       </c>
-      <c r="E13" s="5">
-        <f>SUM(E10:E12)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1" s="9"/>
+      <c r="E14">
+        <f>SUM(E11:E13)</f>
+        <v/>
+      </c>
+    </row>
     <row r="15">
-      <c r="A15" s="13" t="inlineStr">
-        <is>
-          <t>TOTAL MONTHLY COST</t>
-        </is>
-      </c>
-      <c r="E15" s="6">
-        <f>E6+E13</f>
+      <c r="A15" s="13" t="n"/>
+      <c r="E15" s="6" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>TOTAL VPC PEERING COST</t>
+        </is>
+      </c>
+      <c r="E16">
+        <f>E7+E14</f>
         <v/>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="7" t="inlineStr">
-        <is>
-          <t>Notes:</t>
-        </is>
-      </c>
+      <c r="A17" s="7" t="n"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>• VPC Peering connection itself is FREE</t>
+          <t>Notes:</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>• 01_same_region: Same AZ data transfer is FREE</t>
+          <t>• VPC Peering connection itself is FREE</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>• 01_same_region: Cross-AZ is $0.01/GB each direction ($0.02 round-trip)</t>
+          <t>• 01_same_region: NO additional peering cost (base network rates apply)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>• 02_different_region: Cross-Region is $0.02/GB (varies $0.02-$0.05 by region pair)</t>
+          <t>• 02_different_region: $0.02/GB (varies $0.02-$0.05 by region pair)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>• Green cells are inputs - modify Data (GB) values</t>
-        </is>
-      </c>
-    </row>
+          <t>• For same-region peering, total cost = Base Network cost only</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>• For cross-region peering, total cost = Base Network + $0.02/GB peering cost</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>• Green cells (Data GB) are inputs - modify as needed</t>
+        </is>
+      </c>
+    </row>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1098,7 +1060,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
@@ -1117,6 +1079,7 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
@@ -1142,15 +1105,14 @@
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Base Network</t>
-        </is>
-      </c>
-      <c r="B4" s="4">
-        <f>'Base Network'!F7</f>
-        <v/>
+          <t>Base Network (zone-to-zone)</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="C4" s="4">
-        <f>'Base Network'!E15</f>
+        <f>'Base Network'!E8</f>
         <v/>
       </c>
       <c r="D4" s="4">
@@ -1161,15 +1123,15 @@
     <row r="5">
       <c r="A5" s="11" t="inlineStr">
         <is>
-          <t>VPC Peering</t>
+          <t>VPC Peering (component cost)</t>
         </is>
       </c>
       <c r="B5" s="4">
-        <f>'VPC Peering'!E6</f>
+        <f>'VPC Peering'!E7</f>
         <v/>
       </c>
       <c r="C5" s="4">
-        <f>'VPC Peering'!E13</f>
+        <f>'VPC Peering'!E14</f>
         <v/>
       </c>
       <c r="D5" s="4">
@@ -1177,24 +1139,45 @@
         <v/>
       </c>
     </row>
+    <row r="6"/>
     <row r="7" ht="15.75" customHeight="1" s="9">
       <c r="A7" s="13" t="inlineStr">
         <is>
           <t>GRAND TOTAL</t>
         </is>
       </c>
-      <c r="B7" s="14" t="n"/>
-      <c r="C7" s="15" t="n"/>
       <c r="D7" s="6">
         <f>SUM(D4:D5)</f>
         <v/>
       </c>
     </row>
+    <row r="8"/>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Example Calculations:</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>• Same-region VPC Peering: Pay Base Network only</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>• Cross-region VPC Peering: Pay Base Network + VPC Peering cross-region cost</t>
+        </is>
+      </c>
+    </row>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A7:C7"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>